<commit_message>
Add questionnaire PDF and update analysis data
</commit_message>
<xml_diff>
--- a/data/analysis.xlsx
+++ b/data/analysis.xlsx
@@ -1050,7 +1050,7 @@
     <t xml:space="preserve">Improve the product roadmap</t>
   </si>
   <si>
-    <t xml:space="preserve">INFORMALLY (without a prescribed process)</t>
+    <t xml:space="preserve">INFORMALLY (without a prescribed process for carrying out the activity).</t>
   </si>
   <si>
     <t xml:space="preserve">Summarize the product roadmap for stakeholders</t>
@@ -1105,13 +1105,13 @@
     </font>
     <font>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1159,14 +1159,14 @@
       <right style="none"/>
       <top style="none"/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="none"/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="none"/>
       <bottom style="none"/>
@@ -1174,25 +1174,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="none"/>
       <bottom style="none"/>
@@ -1202,10 +1202,10 @@
       <left style="none"/>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -1796,7 +1796,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F56" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="13">
-        <f>(C5/70)*100</f>
+        <f t="shared" ref="D5:D9" si="0">(C5/70)*100</f>
         <v>0</v>
       </c>
       <c r="E5" s="14"/>
@@ -2099,7 +2099,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="13">
-        <f>(G5/56)*100</f>
+        <f t="shared" ref="H5:H9" si="1">(G5/56)*100</f>
         <v>25</v>
       </c>
       <c r="I5" s="14"/>
@@ -2110,7 +2110,7 @@
         <v>23</v>
       </c>
       <c r="L5" s="19">
-        <f>(K5/49)*100</f>
+        <f t="shared" ref="L5:L9" si="2">(K5/49)*100</f>
         <v>46.938775510204081</v>
       </c>
       <c r="M5" s="14"/>
@@ -2118,11 +2118,11 @@
         <v>18</v>
       </c>
       <c r="O5" s="18">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P5" s="13">
-        <f>(O5/33)*100</f>
-        <v>51.515151515151516</v>
+        <f t="shared" ref="P5:P9" si="3">(O5/33)*100</f>
+        <v>45.454545454545453</v>
       </c>
       <c r="Q5" s="14"/>
       <c r="R5" s="18" t="s">
@@ -2132,7 +2132,7 @@
         <v>15</v>
       </c>
       <c r="T5" s="13">
-        <f>(S5/32)*100</f>
+        <f t="shared" ref="T5:T8" si="4">(S5/32)*100</f>
         <v>46.875</v>
       </c>
       <c r="U5" s="1"/>
@@ -2187,7 +2187,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="13">
-        <f>(C6/70)*100</f>
+        <f t="shared" si="0"/>
         <v>54.285714285714285</v>
       </c>
       <c r="E6" s="14"/>
@@ -2198,7 +2198,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="13">
-        <f>(G6/56)*100</f>
+        <f t="shared" si="1"/>
         <v>17.857142857142858</v>
       </c>
       <c r="I6" s="14"/>
@@ -2209,7 +2209,7 @@
         <v>6</v>
       </c>
       <c r="L6" s="19">
-        <f>(K6/49)*100</f>
+        <f t="shared" si="2"/>
         <v>12.244897959183673</v>
       </c>
       <c r="M6" s="14"/>
@@ -2217,11 +2217,11 @@
         <v>28</v>
       </c>
       <c r="O6" s="18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P6" s="13">
-        <f>(O6/33)*100</f>
-        <v>18.181818181818183</v>
+        <f t="shared" si="3"/>
+        <v>21.212121212121211</v>
       </c>
       <c r="Q6" s="14"/>
       <c r="R6" s="18" t="s">
@@ -2231,7 +2231,7 @@
         <v>16</v>
       </c>
       <c r="T6" s="13">
-        <f>(S6/32)*100</f>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="U6" s="1"/>
@@ -2286,7 +2286,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="13">
-        <f>(C7/70)*100</f>
+        <f t="shared" si="0"/>
         <v>28.571428571428569</v>
       </c>
       <c r="E7" s="14"/>
@@ -2297,7 +2297,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="13">
-        <f>(G7/56)*100</f>
+        <f t="shared" si="1"/>
         <v>16.071428571428573</v>
       </c>
       <c r="I7" s="14"/>
@@ -2308,7 +2308,7 @@
         <v>4</v>
       </c>
       <c r="L7" s="19">
-        <f>(K7/49)*100</f>
+        <f t="shared" si="2"/>
         <v>8.1632653061224492</v>
       </c>
       <c r="M7" s="14"/>
@@ -2316,11 +2316,11 @@
         <v>38</v>
       </c>
       <c r="O7" s="18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P7" s="13">
-        <f>(O7/33)*100</f>
-        <v>21.212121212121211</v>
+        <f t="shared" si="3"/>
+        <v>9.0909090909090917</v>
       </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="18" t="s">
@@ -2330,7 +2330,7 @@
         <v>1</v>
       </c>
       <c r="T7" s="13">
-        <f>(S7/32)*100</f>
+        <f t="shared" si="4"/>
         <v>3.125</v>
       </c>
       <c r="U7" s="1"/>
@@ -2385,7 +2385,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="13">
-        <f>(C8/70)*100</f>
+        <f t="shared" si="0"/>
         <v>14.285714285714285</v>
       </c>
       <c r="E8" s="14"/>
@@ -2396,7 +2396,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="13">
-        <f>(G8/56)*100</f>
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="I8" s="14"/>
@@ -2407,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="19">
-        <f>(K8/49)*100</f>
+        <f t="shared" si="2"/>
         <v>6.1224489795918364</v>
       </c>
       <c r="M8" s="14"/>
@@ -2415,11 +2415,11 @@
         <v>47</v>
       </c>
       <c r="O8" s="18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="P8" s="13">
-        <f>(O8/33)*100</f>
-        <v>9.0909090909090917</v>
+        <f t="shared" si="3"/>
+        <v>21.212121212121211</v>
       </c>
       <c r="Q8" s="14"/>
       <c r="R8" s="18" t="s">
@@ -2429,7 +2429,7 @@
         <v>32</v>
       </c>
       <c r="T8" s="13">
-        <f>(S8/32)*100</f>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="U8" s="1"/>
@@ -2484,7 +2484,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="13">
-        <f>(C9/70)*100</f>
+        <f t="shared" si="0"/>
         <v>2.8571428571428572</v>
       </c>
       <c r="E9" s="14"/>
@@ -2495,7 +2495,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="13">
-        <f>(G9/56)*100</f>
+        <f t="shared" si="1"/>
         <v>7.1428571428571423</v>
       </c>
       <c r="I9" s="14"/>
@@ -2506,7 +2506,7 @@
         <v>2</v>
       </c>
       <c r="L9" s="19">
-        <f>(K9/49)*100</f>
+        <f t="shared" si="2"/>
         <v>4.0816326530612246</v>
       </c>
       <c r="M9" s="14"/>
@@ -2514,11 +2514,11 @@
         <v>57</v>
       </c>
       <c r="O9" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="13">
-        <f>(O9/33)*100</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3.0303030303030303</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -2587,7 +2587,7 @@
         <v>3</v>
       </c>
       <c r="H10" s="13">
-        <f>(G10/56)*100</f>
+        <f t="shared" ref="H10:H38" si="5">(G10/56)*100</f>
         <v>5.3571428571428568</v>
       </c>
       <c r="I10" s="14"/>
@@ -2598,7 +2598,7 @@
         <v>2</v>
       </c>
       <c r="L10" s="19">
-        <f>(K10/49)*100</f>
+        <f t="shared" ref="L10:L72" si="6">(K10/49)*100</f>
         <v>4.0816326530612246</v>
       </c>
       <c r="M10" s="14"/>
@@ -2661,7 +2661,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="13">
-        <f>(G11/56)*100</f>
+        <f t="shared" si="5"/>
         <v>3.5714285714285712</v>
       </c>
       <c r="I11" s="14"/>
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="19">
-        <f>(K11/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M11" s="1"/>
@@ -2727,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="13">
-        <f>(G12/56)*100</f>
+        <f t="shared" si="5"/>
         <v>1.7857142857142856</v>
       </c>
       <c r="I12" s="14"/>
@@ -2738,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="19">
-        <f>(K12/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M12" s="14"/>
@@ -2827,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="13">
-        <f>(G13/56)*100</f>
+        <f t="shared" si="5"/>
         <v>1.7857142857142856</v>
       </c>
       <c r="I13" s="14"/>
@@ -2838,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="19">
-        <f>(K13/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M13" s="14"/>
@@ -2849,7 +2849,7 @@
         <v>20</v>
       </c>
       <c r="P13" s="13">
-        <f>(O13/33)*100</f>
+        <f t="shared" ref="P13:P76" si="7">(O13/33)*100</f>
         <v>60.606060606060609</v>
       </c>
       <c r="Q13" s="14"/>
@@ -2920,7 +2920,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="13">
-        <f>(C14/70)*100</f>
+        <f t="shared" ref="D14:D20" si="8">(C14/70)*100</f>
         <v>2.8571428571428572</v>
       </c>
       <c r="E14" s="14"/>
@@ -2931,7 +2931,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="13">
-        <f>(G14/56)*100</f>
+        <f t="shared" si="5"/>
         <v>1.7857142857142856</v>
       </c>
       <c r="I14" s="14"/>
@@ -2942,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="19">
-        <f>(K14/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M14" s="14"/>
@@ -2953,7 +2953,7 @@
         <v>7</v>
       </c>
       <c r="P14" s="13">
-        <f>(O14/33)*100</f>
+        <f t="shared" si="7"/>
         <v>21.212121212121211</v>
       </c>
       <c r="Q14" s="14"/>
@@ -3024,7 +3024,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="13">
-        <f>(C15/70)*100</f>
+        <f t="shared" si="8"/>
         <v>28.571428571428569</v>
       </c>
       <c r="E15" s="14"/>
@@ -3035,7 +3035,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="13">
-        <f>(G15/56)*100</f>
+        <f t="shared" si="5"/>
         <v>1.7857142857142856</v>
       </c>
       <c r="I15" s="14"/>
@@ -3046,7 +3046,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="19">
-        <f>(K15/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M15" s="14"/>
@@ -3057,7 +3057,7 @@
         <v>5</v>
       </c>
       <c r="P15" s="13">
-        <f>(O15/33)*100</f>
+        <f t="shared" si="7"/>
         <v>15.151515151515152</v>
       </c>
       <c r="Q15" s="14"/>
@@ -3128,7 +3128,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="13">
-        <f>(C16/70)*100</f>
+        <f t="shared" si="8"/>
         <v>24.285714285714285</v>
       </c>
       <c r="E16" s="14"/>
@@ -3139,7 +3139,7 @@
         <v>1</v>
       </c>
       <c r="H16" s="13">
-        <f>(G16/56)*100</f>
+        <f t="shared" si="5"/>
         <v>1.7857142857142856</v>
       </c>
       <c r="I16" s="14"/>
@@ -3150,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="19">
-        <f>(K16/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M16" s="14"/>
@@ -3161,7 +3161,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="13">
-        <f>(O16/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q16" s="14"/>
@@ -3232,7 +3232,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="13">
-        <f>(C17/70)*100</f>
+        <f t="shared" si="8"/>
         <v>24.285714285714285</v>
       </c>
       <c r="E17" s="14"/>
@@ -3243,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="13">
-        <f>(G17/56)*100</f>
+        <f t="shared" si="5"/>
         <v>1.7857142857142856</v>
       </c>
       <c r="I17" s="14"/>
@@ -3254,7 +3254,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="19">
-        <f>(K17/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M17" s="14"/>
@@ -3266,7 +3266,7 @@
         <v>33</v>
       </c>
       <c r="P17" s="13">
-        <f>(O17/33)*100</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="Q17" s="14"/>
@@ -3331,7 +3331,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="13">
-        <f>(C18/70)*100</f>
+        <f t="shared" si="8"/>
         <v>14.285714285714285</v>
       </c>
       <c r="E18" s="14"/>
@@ -3342,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="13">
-        <f>(G18/56)*100</f>
+        <f t="shared" si="5"/>
         <v>1.7857142857142856</v>
       </c>
       <c r="I18" s="14"/>
@@ -3353,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="19">
-        <f>(K18/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M18" s="1"/>
@@ -3404,7 +3404,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="13">
-        <f>(C19/70)*100</f>
+        <f t="shared" si="8"/>
         <v>5.7142857142857144</v>
       </c>
       <c r="E19" s="14"/>
@@ -3415,7 +3415,7 @@
         <v>56</v>
       </c>
       <c r="H19" s="13">
-        <f>(G19/56)*100</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="I19" s="14"/>
@@ -3426,7 +3426,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="19">
-        <f>(K19/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M19" s="1"/>
@@ -3471,7 +3471,7 @@
         <v>70</v>
       </c>
       <c r="D20" s="13">
-        <f>(C20/70)*100</f>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="E20" s="1"/>
@@ -3485,7 +3485,7 @@
         <v>49</v>
       </c>
       <c r="L20" s="19">
-        <f>(K20/49)*100</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="M20" s="14"/>
@@ -3561,7 +3561,7 @@
         <v>33</v>
       </c>
       <c r="P21" s="13">
-        <f>(O21/33)*100</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="Q21" s="14"/>
@@ -3580,10 +3580,10 @@
         <v>40</v>
       </c>
       <c r="Z21" s="20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AA21" s="21">
-        <v>0.56299999999999994</v>
+        <v>0.53120000000000001</v>
       </c>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
@@ -3642,7 +3642,7 @@
         <v>27</v>
       </c>
       <c r="P22" s="13">
-        <f>(O22/33)*100</f>
+        <f t="shared" si="7"/>
         <v>81.818181818181827</v>
       </c>
       <c r="Q22" s="14"/>
@@ -3664,7 +3664,7 @@
         <v>9</v>
       </c>
       <c r="AA22" s="21">
-        <v>0.28100000000000003</v>
+        <v>0.28120000000000001</v>
       </c>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
@@ -3725,7 +3725,7 @@
         <v>24</v>
       </c>
       <c r="L23" s="19">
-        <f>(K23/49)*100</f>
+        <f t="shared" si="6"/>
         <v>48.979591836734691</v>
       </c>
       <c r="M23" s="14"/>
@@ -3736,7 +3736,7 @@
         <v>22</v>
       </c>
       <c r="P23" s="13">
-        <f>(O23/33)*100</f>
+        <f t="shared" si="7"/>
         <v>66.666666666666657</v>
       </c>
       <c r="Q23" s="14"/>
@@ -3758,7 +3758,7 @@
         <v>3</v>
       </c>
       <c r="AA23" s="21">
-        <v>0.094</v>
+        <v>0.093699999999999992</v>
       </c>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
@@ -3799,7 +3799,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="19">
-        <f>(C24/70)*100</f>
+        <f t="shared" ref="D24:D60" si="9">(C24/70)*100</f>
         <v>11.428571428571429</v>
       </c>
       <c r="E24" s="14"/>
@@ -3810,7 +3810,7 @@
         <v>10</v>
       </c>
       <c r="H24" s="13">
-        <f>(G24/56)*100</f>
+        <f t="shared" si="5"/>
         <v>17.857142857142858</v>
       </c>
       <c r="I24" s="14"/>
@@ -3821,7 +3821,7 @@
         <v>9</v>
       </c>
       <c r="L24" s="19">
-        <f>(K24/49)*100</f>
+        <f t="shared" si="6"/>
         <v>18.367346938775512</v>
       </c>
       <c r="M24" s="14"/>
@@ -3832,7 +3832,7 @@
         <v>9</v>
       </c>
       <c r="P24" s="13">
-        <f>(O24/33)*100</f>
+        <f t="shared" si="7"/>
         <v>27.27272727272727</v>
       </c>
       <c r="Q24" s="14"/>
@@ -3854,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="AA24" s="21">
-        <v>0.031</v>
+        <v>0.031200000000000002</v>
       </c>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
@@ -3895,7 +3895,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="19">
-        <f>(C25/70)*100</f>
+        <f t="shared" si="9"/>
         <v>24.285714285714285</v>
       </c>
       <c r="E25" s="14"/>
@@ -3906,7 +3906,7 @@
         <v>6</v>
       </c>
       <c r="H25" s="13">
-        <f>(G25/56)*100</f>
+        <f t="shared" si="5"/>
         <v>10.714285714285714</v>
       </c>
       <c r="I25" s="14"/>
@@ -3917,7 +3917,7 @@
         <v>5</v>
       </c>
       <c r="L25" s="19">
-        <f>(K25/49)*100</f>
+        <f t="shared" si="6"/>
         <v>10.204081632653061</v>
       </c>
       <c r="M25" s="14"/>
@@ -3928,7 +3928,7 @@
         <v>9</v>
       </c>
       <c r="P25" s="13">
-        <f>(O25/33)*100</f>
+        <f t="shared" si="7"/>
         <v>27.27272727272727</v>
       </c>
       <c r="Q25" s="14"/>
@@ -3947,10 +3947,10 @@
         <v>49</v>
       </c>
       <c r="Z25" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA25" s="21">
-        <v>0.031</v>
+        <v>0.0625</v>
       </c>
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
@@ -3991,7 +3991,7 @@
         <v>31</v>
       </c>
       <c r="D26" s="19">
-        <f>(C26/70)*100</f>
+        <f t="shared" si="9"/>
         <v>44.285714285714285</v>
       </c>
       <c r="E26" s="14"/>
@@ -4002,7 +4002,7 @@
         <v>9</v>
       </c>
       <c r="H26" s="13">
-        <f>(G26/56)*100</f>
+        <f t="shared" si="5"/>
         <v>16.071428571428573</v>
       </c>
       <c r="I26" s="14"/>
@@ -4013,7 +4013,7 @@
         <v>4</v>
       </c>
       <c r="L26" s="19">
-        <f>(K26/49)*100</f>
+        <f t="shared" si="6"/>
         <v>8.1632653061224492</v>
       </c>
       <c r="M26" s="14"/>
@@ -4024,7 +4024,7 @@
         <v>4</v>
       </c>
       <c r="P26" s="13">
-        <f>(O26/33)*100</f>
+        <f t="shared" si="7"/>
         <v>12.121212121212121</v>
       </c>
       <c r="Q26" s="14"/>
@@ -4069,7 +4069,7 @@
         <v>4</v>
       </c>
       <c r="D27" s="19">
-        <f>(C27/70)*100</f>
+        <f t="shared" si="9"/>
         <v>5.7142857142857144</v>
       </c>
       <c r="E27" s="14"/>
@@ -4080,7 +4080,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="13">
-        <f>(G27/56)*100</f>
+        <f t="shared" si="5"/>
         <v>8.9285714285714288</v>
       </c>
       <c r="I27" s="14"/>
@@ -4091,7 +4091,7 @@
         <v>4</v>
       </c>
       <c r="L27" s="19">
-        <f>(K27/49)*100</f>
+        <f t="shared" si="6"/>
         <v>8.1632653061224492</v>
       </c>
       <c r="M27" s="14"/>
@@ -4102,7 +4102,7 @@
         <v>4</v>
       </c>
       <c r="P27" s="13">
-        <f>(O27/33)*100</f>
+        <f t="shared" si="7"/>
         <v>12.121212121212121</v>
       </c>
       <c r="Q27" s="14"/>
@@ -4147,7 +4147,7 @@
         <v>10</v>
       </c>
       <c r="D28" s="19">
-        <f>(C28/70)*100</f>
+        <f t="shared" si="9"/>
         <v>14.285714285714285</v>
       </c>
       <c r="E28" s="14"/>
@@ -4158,7 +4158,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="13">
-        <f>(G28/56)*100</f>
+        <f t="shared" si="5"/>
         <v>3.5714285714285712</v>
       </c>
       <c r="I28" s="14"/>
@@ -4169,7 +4169,7 @@
         <v>1</v>
       </c>
       <c r="L28" s="19">
-        <f>(K28/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M28" s="14"/>
@@ -4180,7 +4180,7 @@
         <v>2</v>
       </c>
       <c r="P28" s="13">
-        <f>(O28/33)*100</f>
+        <f t="shared" si="7"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="Q28" s="1"/>
@@ -4233,7 +4233,7 @@
         <v>70</v>
       </c>
       <c r="D29" s="19">
-        <f>(C29/70)*100</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="E29" s="14"/>
@@ -4244,7 +4244,7 @@
         <v>6</v>
       </c>
       <c r="H29" s="13">
-        <f>(G29/56)*100</f>
+        <f t="shared" si="5"/>
         <v>10.714285714285714</v>
       </c>
       <c r="I29" s="14"/>
@@ -4255,7 +4255,7 @@
         <v>1</v>
       </c>
       <c r="L29" s="19">
-        <f>(K29/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M29" s="14"/>
@@ -4266,7 +4266,7 @@
         <v>1</v>
       </c>
       <c r="P29" s="13">
-        <f>(O29/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q29" s="1"/>
@@ -4323,7 +4323,7 @@
         <v>6</v>
       </c>
       <c r="H30" s="13">
-        <f>(G30/56)*100</f>
+        <f t="shared" si="5"/>
         <v>10.714285714285714</v>
       </c>
       <c r="I30" s="14"/>
@@ -4334,7 +4334,7 @@
         <v>1</v>
       </c>
       <c r="L30" s="19">
-        <f>(K30/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M30" s="14"/>
@@ -4345,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="P30" s="13">
-        <f>(O30/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q30" s="14"/>
@@ -4414,7 +4414,7 @@
         <v>6</v>
       </c>
       <c r="H31" s="13">
-        <f>(G31/56)*100</f>
+        <f t="shared" si="5"/>
         <v>10.714285714285714</v>
       </c>
       <c r="I31" s="14"/>
@@ -4425,7 +4425,7 @@
         <v>49</v>
       </c>
       <c r="L31" s="19">
-        <f>(K31/49)*100</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="M31" s="14"/>
@@ -4436,7 +4436,7 @@
         <v>1</v>
       </c>
       <c r="P31" s="13">
-        <f>(O31/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q31" s="14"/>
@@ -4505,7 +4505,7 @@
         <v>6</v>
       </c>
       <c r="H32" s="13">
-        <f>(G32/56)*100</f>
+        <f t="shared" si="5"/>
         <v>10.714285714285714</v>
       </c>
       <c r="I32" s="1"/>
@@ -4520,7 +4520,7 @@
         <v>1</v>
       </c>
       <c r="P32" s="13">
-        <f>(O32/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q32" s="14"/>
@@ -4579,7 +4579,7 @@
         <v>14</v>
       </c>
       <c r="D33" s="29">
-        <f>(C33/70)*100</f>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="E33" s="14"/>
@@ -4591,7 +4591,7 @@
         <v>56</v>
       </c>
       <c r="H33" s="13">
-        <f>(G33/56)*100</f>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="I33" s="1"/>
@@ -4606,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="P33" s="13">
-        <f>(O33/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q33" s="14"/>
@@ -4665,7 +4665,7 @@
         <v>20</v>
       </c>
       <c r="D34" s="13">
-        <f>(C34/70)*100</f>
+        <f t="shared" si="9"/>
         <v>28.571428571428569</v>
       </c>
       <c r="E34" s="1"/>
@@ -4690,7 +4690,7 @@
         <v>1</v>
       </c>
       <c r="P34" s="13">
-        <f>(O34/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q34" s="14"/>
@@ -4749,7 +4749,7 @@
         <v>22</v>
       </c>
       <c r="D35" s="13">
-        <f>(C35/70)*100</f>
+        <f t="shared" si="9"/>
         <v>31.428571428571427</v>
       </c>
       <c r="E35" s="1"/>
@@ -4764,7 +4764,7 @@
         <v>10</v>
       </c>
       <c r="L35" s="19">
-        <f>(K35/49)*100</f>
+        <f t="shared" si="6"/>
         <v>20.408163265306122</v>
       </c>
       <c r="M35" s="1"/>
@@ -4827,7 +4827,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="13">
-        <f>(C36/70)*100</f>
+        <f t="shared" si="9"/>
         <v>14.285714285714285</v>
       </c>
       <c r="E36" s="14"/>
@@ -4848,7 +4848,7 @@
         <v>9</v>
       </c>
       <c r="L36" s="19">
-        <f>(K36/49)*100</f>
+        <f t="shared" si="6"/>
         <v>18.367346938775512</v>
       </c>
       <c r="M36" s="1"/>
@@ -4899,7 +4899,7 @@
         <v>4</v>
       </c>
       <c r="D37" s="13">
-        <f>(C37/70)*100</f>
+        <f t="shared" si="9"/>
         <v>5.7142857142857144</v>
       </c>
       <c r="E37" s="14"/>
@@ -4910,7 +4910,7 @@
         <v>49</v>
       </c>
       <c r="H37" s="29">
-        <f>(G37/56)*100</f>
+        <f t="shared" si="5"/>
         <v>87.5</v>
       </c>
       <c r="I37" s="14"/>
@@ -4921,7 +4921,7 @@
         <v>8</v>
       </c>
       <c r="L37" s="19">
-        <f>(K37/49)*100</f>
+        <f t="shared" si="6"/>
         <v>16.326530612244898</v>
       </c>
       <c r="M37" s="14"/>
@@ -4978,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="13">
-        <f>(C38/70)*100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E38" s="14"/>
@@ -4989,7 +4989,7 @@
         <v>7</v>
       </c>
       <c r="H38" s="13">
-        <f>(G38/56)*100</f>
+        <f t="shared" si="5"/>
         <v>12.5</v>
       </c>
       <c r="I38" s="14"/>
@@ -5000,7 +5000,7 @@
         <v>5</v>
       </c>
       <c r="L38" s="19">
-        <f>(K38/49)*100</f>
+        <f t="shared" si="6"/>
         <v>10.204081632653061</v>
       </c>
       <c r="M38" s="14"/>
@@ -5011,7 +5011,7 @@
         <v>9</v>
       </c>
       <c r="P38" s="13">
-        <f>(O38/33)*100</f>
+        <f t="shared" si="7"/>
         <v>27.27272727272727</v>
       </c>
       <c r="Q38" s="14"/>
@@ -5070,7 +5070,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="13">
-        <f>(C39/70)*100</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E39" s="1"/>
@@ -5085,7 +5085,7 @@
         <v>4</v>
       </c>
       <c r="L39" s="19">
-        <f>(K39/49)*100</f>
+        <f t="shared" si="6"/>
         <v>8.1632653061224492</v>
       </c>
       <c r="M39" s="14"/>
@@ -5096,7 +5096,7 @@
         <v>7</v>
       </c>
       <c r="P39" s="13">
-        <f>(O39/33)*100</f>
+        <f t="shared" si="7"/>
         <v>21.212121212121211</v>
       </c>
       <c r="Q39" s="14"/>
@@ -5155,7 +5155,7 @@
         <v>70</v>
       </c>
       <c r="D40" s="13">
-        <f>(C40/70)*100</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="E40" s="1"/>
@@ -5170,7 +5170,7 @@
         <v>3</v>
       </c>
       <c r="L40" s="19">
-        <f>(K40/49)*100</f>
+        <f t="shared" si="6"/>
         <v>6.1224489795918364</v>
       </c>
       <c r="M40" s="14"/>
@@ -5181,7 +5181,7 @@
         <v>5</v>
       </c>
       <c r="P40" s="13">
-        <f>(O40/33)*100</f>
+        <f t="shared" si="7"/>
         <v>15.151515151515152</v>
       </c>
       <c r="Q40" s="14"/>
@@ -5242,7 +5242,7 @@
         <v>2</v>
       </c>
       <c r="L41" s="19">
-        <f>(K41/49)*100</f>
+        <f t="shared" si="6"/>
         <v>4.0816326530612246</v>
       </c>
       <c r="M41" s="14"/>
@@ -5253,7 +5253,7 @@
         <v>4</v>
       </c>
       <c r="P41" s="13">
-        <f>(O41/33)*100</f>
+        <f t="shared" si="7"/>
         <v>12.121212121212121</v>
       </c>
       <c r="Q41" s="14"/>
@@ -5314,7 +5314,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="19">
-        <f>(K42/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M42" s="14"/>
@@ -5325,7 +5325,7 @@
         <v>2</v>
       </c>
       <c r="P42" s="13">
-        <f>(O42/33)*100</f>
+        <f t="shared" si="7"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="Q42" s="14"/>
@@ -5398,7 +5398,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="19">
-        <f>(K43/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M43" s="14"/>
@@ -5409,7 +5409,7 @@
         <v>1</v>
       </c>
       <c r="P43" s="13">
-        <f>(O43/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q43" s="14"/>
@@ -5468,7 +5468,7 @@
         <v>16</v>
       </c>
       <c r="D44" s="13">
-        <f>(C44/70)*100</f>
+        <f t="shared" si="9"/>
         <v>22.857142857142858</v>
       </c>
       <c r="E44" s="1"/>
@@ -5483,7 +5483,7 @@
         <v>1</v>
       </c>
       <c r="L44" s="19">
-        <f>(K44/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M44" s="14"/>
@@ -5494,7 +5494,7 @@
         <v>2</v>
       </c>
       <c r="P44" s="13">
-        <f>(O44/33)*100</f>
+        <f t="shared" si="7"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="Q44" s="14"/>
@@ -5553,7 +5553,7 @@
         <v>4</v>
       </c>
       <c r="D45" s="13">
-        <f>(C45/70)*100</f>
+        <f t="shared" si="9"/>
         <v>5.7142857142857144</v>
       </c>
       <c r="E45" s="1"/>
@@ -5568,7 +5568,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="19">
-        <f>(K45/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M45" s="14"/>
@@ -5579,7 +5579,7 @@
         <v>1</v>
       </c>
       <c r="P45" s="13">
-        <f>(O45/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q45" s="14"/>
@@ -5632,7 +5632,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="13">
-        <f>(C46/70)*100</f>
+        <f t="shared" si="9"/>
         <v>2.8571428571428572</v>
       </c>
       <c r="E46" s="1"/>
@@ -5647,7 +5647,7 @@
         <v>1</v>
       </c>
       <c r="L46" s="19">
-        <f>(K46/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M46" s="14"/>
@@ -5658,7 +5658,7 @@
         <v>2</v>
       </c>
       <c r="P46" s="13">
-        <f>(O46/33)*100</f>
+        <f t="shared" si="7"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="Q46" s="14"/>
@@ -5725,7 +5725,7 @@
         <v>10</v>
       </c>
       <c r="D47" s="13">
-        <f>(C47/70)*100</f>
+        <f t="shared" si="9"/>
         <v>14.285714285714285</v>
       </c>
       <c r="E47" s="1"/>
@@ -5740,7 +5740,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="19">
-        <f>(K47/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M47" s="14"/>
@@ -5751,7 +5751,7 @@
         <v>1</v>
       </c>
       <c r="P47" s="13">
-        <f>(O47/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q47" s="14"/>
@@ -5818,7 +5818,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="13">
-        <f>(C48/70)*100</f>
+        <f t="shared" si="9"/>
         <v>5.7142857142857144</v>
       </c>
       <c r="E48" s="1"/>
@@ -5833,7 +5833,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="19">
-        <f>(K48/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M48" s="14"/>
@@ -5844,7 +5844,7 @@
         <v>1</v>
       </c>
       <c r="P48" s="13">
-        <f>(O48/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q48" s="14"/>
@@ -5911,7 +5911,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="13">
-        <f>(C49/70)*100</f>
+        <f t="shared" si="9"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="E49" s="1"/>
@@ -5926,7 +5926,7 @@
         <v>1</v>
       </c>
       <c r="L49" s="19">
-        <f>(K49/49)*100</f>
+        <f t="shared" si="6"/>
         <v>2.0408163265306123</v>
       </c>
       <c r="M49" s="14"/>
@@ -5937,7 +5937,7 @@
         <v>1</v>
       </c>
       <c r="P49" s="13">
-        <f>(O49/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q49" s="14"/>
@@ -6004,7 +6004,7 @@
         <v>42</v>
       </c>
       <c r="D50" s="13">
-        <f>(C50/70)*100</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="E50" s="1"/>
@@ -6023,7 +6023,7 @@
         <v>1</v>
       </c>
       <c r="P50" s="13">
-        <f>(O50/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q50" s="14"/>
@@ -6090,7 +6090,7 @@
         <v>70</v>
       </c>
       <c r="D51" s="13">
-        <f>(C51/70)*100</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="E51" s="1"/>
@@ -6115,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="P51" s="13">
-        <f>(O51/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q51" s="14"/>
@@ -6190,7 +6190,7 @@
         <v>15</v>
       </c>
       <c r="L52" s="19">
-        <f>(K52/49)*100</f>
+        <f t="shared" si="6"/>
         <v>30.612244897959183</v>
       </c>
       <c r="M52" s="14"/>
@@ -6201,7 +6201,7 @@
         <v>1</v>
       </c>
       <c r="P52" s="13">
-        <f>(O52/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q52" s="14"/>
@@ -6262,7 +6262,7 @@
         <v>17</v>
       </c>
       <c r="L53" s="19">
-        <f>(K53/49)*100</f>
+        <f t="shared" si="6"/>
         <v>34.693877551020407</v>
       </c>
       <c r="M53" s="14"/>
@@ -6273,7 +6273,7 @@
         <v>2</v>
       </c>
       <c r="P53" s="13">
-        <f>(O53/33)*100</f>
+        <f t="shared" si="7"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="Q53" s="14"/>
@@ -6340,7 +6340,7 @@
         <v>11</v>
       </c>
       <c r="L54" s="19">
-        <f>(K54/49)*100</f>
+        <f t="shared" si="6"/>
         <v>22.448979591836736</v>
       </c>
       <c r="M54" s="1"/>
@@ -6397,7 +6397,7 @@
         <v>15</v>
       </c>
       <c r="D55" s="13">
-        <f>(C55/70)*100</f>
+        <f t="shared" si="9"/>
         <v>21.428571428571427</v>
       </c>
       <c r="E55" s="1"/>
@@ -6412,7 +6412,7 @@
         <v>4</v>
       </c>
       <c r="L55" s="19">
-        <f>(K55/49)*100</f>
+        <f t="shared" si="6"/>
         <v>8.1632653061224492</v>
       </c>
       <c r="M55" s="1"/>
@@ -6469,7 +6469,7 @@
         <v>8</v>
       </c>
       <c r="D56" s="13">
-        <f>(C56/70)*100</f>
+        <f t="shared" si="9"/>
         <v>11.428571428571429</v>
       </c>
       <c r="E56" s="1"/>
@@ -6484,7 +6484,7 @@
         <v>2</v>
       </c>
       <c r="L56" s="19">
-        <f>(K56/49)*100</f>
+        <f t="shared" si="6"/>
         <v>4.0816326530612246</v>
       </c>
       <c r="M56" s="1"/>
@@ -6541,7 +6541,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="13">
-        <f>(C57/70)*100</f>
+        <f t="shared" si="9"/>
         <v>5.7142857142857144</v>
       </c>
       <c r="E57" s="1"/>
@@ -6556,7 +6556,7 @@
         <v>49</v>
       </c>
       <c r="L57" s="19">
-        <f>(K57/49)*100</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="M57" s="14"/>
@@ -6619,7 +6619,7 @@
         <v>2</v>
       </c>
       <c r="D58" s="13">
-        <f>(C58/70)*100</f>
+        <f t="shared" si="9"/>
         <v>2.8571428571428572</v>
       </c>
       <c r="E58" s="1"/>
@@ -6638,7 +6638,7 @@
         <v>33</v>
       </c>
       <c r="P58" s="13">
-        <f>(O58/33)*100</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="Q58" s="14"/>
@@ -6691,7 +6691,7 @@
         <v>47</v>
       </c>
       <c r="D59" s="13">
-        <f>(C59/70)*100</f>
+        <f t="shared" si="9"/>
         <v>67.142857142857139</v>
       </c>
       <c r="E59" s="1"/>
@@ -6710,7 +6710,7 @@
         <v>25</v>
       </c>
       <c r="P59" s="13">
-        <f>(O59/33)*100</f>
+        <f t="shared" si="7"/>
         <v>75.757575757575751</v>
       </c>
       <c r="Q59" s="1"/>
@@ -6751,7 +6751,7 @@
         <v>70</v>
       </c>
       <c r="D60" s="13">
-        <f>(C60/70)*100</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="E60" s="1"/>
@@ -6776,7 +6776,7 @@
         <v>20</v>
       </c>
       <c r="P60" s="13">
-        <f>(O60/33)*100</f>
+        <f t="shared" si="7"/>
         <v>60.606060606060609</v>
       </c>
       <c r="Q60" s="1"/>
@@ -6825,7 +6825,7 @@
         <v>12</v>
       </c>
       <c r="L61" s="19">
-        <f>(K61/49)*100</f>
+        <f t="shared" si="6"/>
         <v>24.489795918367346</v>
       </c>
       <c r="M61" s="14"/>
@@ -6836,7 +6836,7 @@
         <v>18</v>
       </c>
       <c r="P61" s="13">
-        <f>(O61/33)*100</f>
+        <f t="shared" si="7"/>
         <v>54.54545454545454</v>
       </c>
       <c r="Q61" s="14"/>
@@ -6891,7 +6891,7 @@
         <v>14</v>
       </c>
       <c r="L62" s="19">
-        <f>(K62/49)*100</f>
+        <f t="shared" si="6"/>
         <v>28.571428571428569</v>
       </c>
       <c r="M62" s="14"/>
@@ -6902,7 +6902,7 @@
         <v>2</v>
       </c>
       <c r="P62" s="13">
-        <f>(O62/33)*100</f>
+        <f t="shared" si="7"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="Q62" s="14"/>
@@ -6957,7 +6957,7 @@
         <v>6</v>
       </c>
       <c r="L63" s="19">
-        <f>(K63/49)*100</f>
+        <f t="shared" si="6"/>
         <v>12.244897959183673</v>
       </c>
       <c r="M63" s="1"/>
@@ -7016,7 +7016,7 @@
         <v>5</v>
       </c>
       <c r="L64" s="19">
-        <f>(K64/49)*100</f>
+        <f t="shared" si="6"/>
         <v>10.204081632653061</v>
       </c>
       <c r="M64" s="1"/>
@@ -7075,7 +7075,7 @@
         <v>12</v>
       </c>
       <c r="L65" s="19">
-        <f>(K65/49)*100</f>
+        <f t="shared" si="6"/>
         <v>24.489795918367346</v>
       </c>
       <c r="M65" s="14"/>
@@ -7138,7 +7138,7 @@
         <v>49</v>
       </c>
       <c r="L66" s="19">
-        <f>(K66/49)*100</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="M66" s="14"/>
@@ -7149,7 +7149,7 @@
         <v>12</v>
       </c>
       <c r="P66" s="13">
-        <f>(O66/33)*100</f>
+        <f t="shared" si="7"/>
         <v>36.363636363636367</v>
       </c>
       <c r="Q66" s="14"/>
@@ -7208,7 +7208,7 @@
         <v>12</v>
       </c>
       <c r="P67" s="13">
-        <f>(O67/33)*100</f>
+        <f t="shared" si="7"/>
         <v>36.363636363636367</v>
       </c>
       <c r="Q67" s="1"/>
@@ -7261,7 +7261,7 @@
         <v>4</v>
       </c>
       <c r="P68" s="13">
-        <f>(O68/33)*100</f>
+        <f t="shared" si="7"/>
         <v>12.121212121212121</v>
       </c>
       <c r="Q68" s="1"/>
@@ -7320,7 +7320,7 @@
         <v>4</v>
       </c>
       <c r="P69" s="13">
-        <f>(O69/33)*100</f>
+        <f t="shared" si="7"/>
         <v>12.121212121212121</v>
       </c>
       <c r="Q69" s="14"/>
@@ -7381,7 +7381,7 @@
         <v>33</v>
       </c>
       <c r="L70" s="34">
-        <f>(K70/49)*100</f>
+        <f t="shared" si="6"/>
         <v>67.346938775510196</v>
       </c>
       <c r="M70" s="14"/>
@@ -7392,7 +7392,7 @@
         <v>1</v>
       </c>
       <c r="P70" s="13">
-        <f>(O70/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q70" s="14"/>
@@ -7453,7 +7453,7 @@
         <v>16</v>
       </c>
       <c r="L71" s="19">
-        <f>(K71/49)*100</f>
+        <f t="shared" si="6"/>
         <v>32.653061224489797</v>
       </c>
       <c r="M71" s="14"/>
@@ -7464,7 +7464,7 @@
         <v>33</v>
       </c>
       <c r="P71" s="13">
-        <f>(O71/33)*100</f>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="Q71" s="14"/>
@@ -7525,7 +7525,7 @@
         <v>49</v>
       </c>
       <c r="L72" s="19">
-        <f>(K72/49)*100</f>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="M72" s="1"/>
@@ -7653,11 +7653,11 @@
         <v>343</v>
       </c>
       <c r="O74" s="36">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P74" s="37">
-        <f>(O74/33)*100</f>
-        <v>51.515151515151516</v>
+        <f t="shared" si="7"/>
+        <v>48.484848484848484</v>
       </c>
       <c r="Q74" s="14"/>
       <c r="R74" s="18" t="s">
@@ -7718,11 +7718,11 @@
         <v>345</v>
       </c>
       <c r="O75" s="36">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P75" s="37">
-        <f>(O75/33)*100</f>
-        <v>45.454545454545453</v>
+        <f t="shared" si="7"/>
+        <v>48.484848484848484</v>
       </c>
       <c r="Q75" s="14"/>
       <c r="R75" s="18" t="s">
@@ -7786,7 +7786,7 @@
         <v>1</v>
       </c>
       <c r="P76" s="29">
-        <f>(O76/33)*100</f>
+        <f t="shared" si="7"/>
         <v>3.0303030303030303</v>
       </c>
       <c r="Q76" s="14"/>
@@ -7851,7 +7851,7 @@
         <v>33</v>
       </c>
       <c r="P77" s="37">
-        <f>(O77/33)*100</f>
+        <f t="shared" ref="P77" si="10">(O77/33)*100</f>
         <v>100</v>
       </c>
       <c r="Q77" s="14"/>
@@ -50679,7 +50679,7 @@
     <mergeCell ref="AN2:AQ2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>

</xml_diff>